<commit_message>
se esta actualizando el cronograma de la configuracion
</commit_message>
<xml_diff>
--- a/Proyectos/BO/Librería de Trabajo/Gestión de Proyecto/BO_C.xlsx
+++ b/Proyectos/BO/Librería de Trabajo/Gestión de Proyecto/BO_C.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repositorio_GIT\G2_ALPHA_BUSINESS\BO\Librería de Trabajo\Gestión de Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repositorio_GIT\G2_ALPHA_BUSINESS\Proyectos\BO\Librería de Trabajo\Gestión de Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,9 +564,7 @@
       <c r="D5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="13">
-        <v>42490</v>
-      </c>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
@@ -625,10 +623,10 @@
         <v>8</v>
       </c>
       <c r="E13" s="12">
-        <v>42455</v>
+        <v>42482</v>
       </c>
       <c r="F13" s="12">
-        <v>42460</v>
+        <v>42490</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
@@ -639,10 +637,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="13">
-        <v>42455</v>
+        <v>42482</v>
       </c>
       <c r="F14" s="13">
-        <v>42456</v>
+        <v>42483</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
@@ -653,10 +651,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="13">
-        <v>42456</v>
+        <v>42483</v>
       </c>
       <c r="F15" s="13">
-        <v>42457</v>
+        <v>42484</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
@@ -667,10 +665,10 @@
         <v>3</v>
       </c>
       <c r="E16" s="13">
-        <v>42456</v>
+        <v>42484</v>
       </c>
       <c r="F16" s="13">
-        <v>42459</v>
+        <v>42487</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
@@ -681,10 +679,10 @@
         <v>2</v>
       </c>
       <c r="E17" s="13">
-        <v>42458</v>
+        <v>42487</v>
       </c>
       <c r="F17" s="13">
-        <v>42460</v>
+        <v>42489</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
@@ -695,10 +693,10 @@
         <v>1</v>
       </c>
       <c r="E18" s="13">
-        <v>42459</v>
+        <v>42489</v>
       </c>
       <c r="F18" s="13">
-        <v>42460</v>
+        <v>42490</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
@@ -706,13 +704,13 @@
         <v>6</v>
       </c>
       <c r="D19" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E19" s="12">
-        <v>42461</v>
+        <v>42490</v>
       </c>
       <c r="F19" s="12">
-        <v>42466</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
@@ -723,10 +721,10 @@
         <v>1</v>
       </c>
       <c r="E20" s="14">
-        <v>42461</v>
+        <v>42490</v>
       </c>
       <c r="F20" s="13">
-        <v>42462</v>
+        <v>42491</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
@@ -734,13 +732,13 @@
         <v>8</v>
       </c>
       <c r="D21" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E21" s="13">
-        <v>42463</v>
+        <v>42491</v>
       </c>
       <c r="F21" s="13">
-        <v>42464</v>
+        <v>42494</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
@@ -751,10 +749,10 @@
         <v>1</v>
       </c>
       <c r="E22" s="13">
-        <v>42465</v>
+        <v>42495</v>
       </c>
       <c r="F22" s="13">
-        <v>42466</v>
+        <v>42496</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>